<commit_message>
New Commit as per Sandbox => 07/12/2020
</commit_message>
<xml_diff>
--- a/rrd/AppData/AccountAllocation.xlsx
+++ b/rrd/AppData/AccountAllocation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\git\RRD_Anshu\rrd\AppData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rai Sigh\git\RRD_Opportunity\rrd\AppData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06C82EE6-8476-4F9C-9997-DCE6830D3A16}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{600F5F34-A4BE-4FCB-AB0A-E2A75CACF426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" firstSheet="9" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" firstSheet="8" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AccountAllocation1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="110">
   <si>
     <t>AccountName</t>
   </si>
@@ -363,23 +363,17 @@
     <t>ToBeAssignedAfterdistribution</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>AccountConfig</t>
   </si>
   <si>
     <t>Accountconfig2</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,6 +403,39 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -446,15 +473,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -741,17 +777,17 @@
       <selection activeCell="G1" sqref="G1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="24.21875" customWidth="1"/>
-    <col min="7" max="7" width="19.21875" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="24.28515625" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,10 +807,10 @@
         <v>24</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -785,7 +821,7 @@
         <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -800,173 +836,173 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H1"/>
+      <selection activeCell="H2" sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="17.44140625" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="31.33203125" customWidth="1"/>
-    <col min="8" max="8" width="29.5546875" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" customWidth="1"/>
+    <col min="7" max="7" width="31.28515625" customWidth="1"/>
+    <col min="8" max="8" width="29.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="H2" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="H3" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="H4" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="H5" s="16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="16" t="s">
         <v>77</v>
       </c>
     </row>
@@ -977,150 +1013,193 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95B52DE-F3A0-4145-81ED-8EA1C3700BFB}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D4" sqref="A1:I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.88671875" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.88671875" customWidth="1"/>
-    <col min="5" max="5" width="21.21875" customWidth="1"/>
-    <col min="6" max="6" width="21.109375" customWidth="1"/>
-    <col min="7" max="7" width="48.109375" customWidth="1"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1"/>
+    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="H1" s="15" t="s">
+        <v>106</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="H2" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>75</v>
+      <c r="F6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1129,144 +1208,148 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F4" sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.77734375" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" customWidth="1"/>
-    <col min="7" max="7" width="48.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="F5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="F6" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1282,17 +1365,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="7" width="49.33203125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="49.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1315,7 +1398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1338,7 +1421,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -1358,7 +1441,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>61</v>
       </c>
@@ -1378,7 +1461,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>102</v>
       </c>
@@ -1398,7 +1481,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>103</v>
       </c>
@@ -1428,19 +1511,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="3" max="3" width="18.33203125" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1543,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1480,7 +1563,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>68</v>
       </c>
@@ -1500,7 +1583,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>69</v>
       </c>
@@ -1520,7 +1603,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -1551,20 +1634,20 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
-    <col min="7" max="7" width="51.21875" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" customWidth="1"/>
+    <col min="7" max="7" width="51.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1587,7 +1670,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1610,7 +1693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1630,7 +1713,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>63</v>
       </c>
@@ -1650,7 +1733,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1670,7 +1753,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>65</v>
       </c>
@@ -1690,7 +1773,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>66</v>
       </c>
@@ -1721,19 +1804,19 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1753,14 +1836,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="4" t="s">
@@ -1773,14 +1856,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>80</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -1793,14 +1876,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>81</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -1813,14 +1896,14 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>82</v>
       </c>
       <c r="B5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -1835,6 +1918,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1846,16 +1930,16 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1875,7 +1959,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1895,7 +1979,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1915,7 +1999,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1935,7 +2019,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1955,7 +2039,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>64</v>
       </c>
@@ -1989,17 +2073,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.88671875" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
-    <col min="6" max="6" width="20.77734375" customWidth="1"/>
-    <col min="7" max="7" width="48.109375" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="48.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2022,7 +2106,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2045,7 +2129,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -2065,7 +2149,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2085,7 +2169,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -2114,128 +2198,130 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20B1DC93-42AB-4214-AA11-E714C2CEC83A}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" customWidth="1"/>
-    <col min="5" max="5" width="18.109375" customWidth="1"/>
-    <col min="6" max="6" width="21.5546875" customWidth="1"/>
-    <col min="7" max="7" width="48.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="F4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>75</v>
-      </c>
+      <c r="F5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G5" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2244,19 +2330,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.21875" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2276,7 +2362,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2296,7 +2382,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -2316,7 +2402,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -2336,7 +2422,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -2356,7 +2442,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -2376,7 +2462,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -2405,204 +2491,203 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDA81170-3C5B-4F53-BAF1-2C80E56ECB4D}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
-    <col min="4" max="4" width="18.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" customWidth="1"/>
-    <col min="7" max="7" width="25.21875" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="H2" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="F3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="H3" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="H4" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H5" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="H5" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="H6" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="11" t="s">
         <v>77</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>